<commit_message>
Update: Update Qt Walkthrough about table
</commit_message>
<xml_diff>
--- a/qt-samples/Windows/qt-table-win10/features/support/data/spreadsheet_data.xlsx
+++ b/qt-samples/Windows/qt-table-win10/features/support/data/spreadsheet_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dream\Documents\LeanPro\文档\Qt自动化测试教程企划案\QtTableProject_Win10\features\support\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dream\Documents\LeanPro\demos\qt-samples\Windows\qt-table-win10\features\support\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9394CF14-AE99-4370-93FD-EFF008137BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94DF0B6-C6AB-46D8-A730-932D1DAD4C32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="1704" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,114 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+  <si>
+    <t>15/6/2006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21/5/2006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16/6/2006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>包子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CNY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>馒头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可乐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>矿泉水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>薯片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
   <si>
     <t>Item</t>
   </si>
@@ -47,35 +154,7 @@
     <t>Currency</t>
   </si>
   <si>
-    <t>Ex.Rate</t>
-  </si>
-  <si>
-    <t>NOK</t>
-  </si>
-  <si>
-    <t>包子</t>
-  </si>
-  <si>
-    <t>CNY</t>
-  </si>
-  <si>
-    <t>馒头</t>
-  </si>
-  <si>
-    <t>可乐</t>
-  </si>
-  <si>
-    <t>矿泉水</t>
-  </si>
-  <si>
-    <t>薯片</t>
-  </si>
-  <si>
-    <t>17/02/2020</t>
-  </si>
-  <si>
-    <t>17/02/2020</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Ex. Rate</t>
   </si>
 </sst>
 </file>
@@ -132,10 +211,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -442,141 +521,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.6328125"/>
-    <col min="6" max="6" width="11.08984375" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
+      <c r="A2" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2">
-        <v>0.8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="F2">
-        <f>C2*E2</f>
-        <v>0.16000000000000003</v>
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
-        <v>0.5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="F3">
-        <f>C3*E3</f>
-        <v>0.1</v>
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>3.5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="F4">
-        <f>C4*E4</f>
-        <v>0.70000000000000007</v>
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="F5">
-        <f>C5*E5</f>
-        <v>0.4</v>
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>6.5</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="F6">
-        <f>C6*E6</f>
-        <v>1.3</v>
       </c>
     </row>
   </sheetData>
@@ -592,7 +686,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -606,7 +700,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>